<commit_message>
Add info through California to bishops spreadsheet.
</commit_message>
<xml_diff>
--- a/Bishops and dioceses.xlsx
+++ b/Bishops and dioceses.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\Data analysis\bishopsAndTwitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58DF85A-22F7-4438-9A63-58EBBB15FA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FBC6D6-56DE-4A7B-B158-1B6279626170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10086" yWindow="300" windowWidth="20634" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10158" yWindow="288" windowWidth="20634" windowHeight="17058" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bishops and dioceses" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="172">
   <si>
     <t>State</t>
   </si>
@@ -287,6 +287,255 @@
   </si>
   <si>
     <t>@bhmcatholic</t>
+  </si>
+  <si>
+    <t>Cordileone</t>
+  </si>
+  <si>
+    <t>Salvatore J.</t>
+  </si>
+  <si>
+    <t>http://www.sfarchdiocese.org/</t>
+  </si>
+  <si>
+    <t>Justice</t>
+  </si>
+  <si>
+    <t>William J.</t>
+  </si>
+  <si>
+    <t>Wang</t>
+  </si>
+  <si>
+    <t>Ignatius C.</t>
+  </si>
+  <si>
+    <t>Fresno</t>
+  </si>
+  <si>
+    <t>Brennan</t>
+  </si>
+  <si>
+    <t>Joseph V.</t>
+  </si>
+  <si>
+    <t>http://www.dioceseoffresno.org/</t>
+  </si>
+  <si>
+    <t>Ochoa</t>
+  </si>
+  <si>
+    <t>Armando X.</t>
+  </si>
+  <si>
+    <t>Monterey</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Daniel E.</t>
+  </si>
+  <si>
+    <t>http://www.dioceseofmonterey.org/</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Sylvester D.</t>
+  </si>
+  <si>
+    <t>Oakland</t>
+  </si>
+  <si>
+    <t>Barber</t>
+  </si>
+  <si>
+    <t>Michael C.</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>http://www.oakdiocese.org/</t>
+  </si>
+  <si>
+    <t>Cummins</t>
+  </si>
+  <si>
+    <t>John S.</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Vann</t>
+  </si>
+  <si>
+    <t>Kevin W.</t>
+  </si>
+  <si>
+    <t>http://www.rcbo.org/</t>
+  </si>
+  <si>
+    <t>Freyer</t>
+  </si>
+  <si>
+    <t>Timothey E.</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Than Thai</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Tod D.</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Soto</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>http://www.diocese-sacramento.org/</t>
+  </si>
+  <si>
+    <t>Weigand</t>
+  </si>
+  <si>
+    <t>William K.</t>
+  </si>
+  <si>
+    <t>San Bernadino</t>
+  </si>
+  <si>
+    <t>Rojas</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>http://www.sbdiocese.org/</t>
+  </si>
+  <si>
+    <t>Barnes</t>
+  </si>
+  <si>
+    <t>Gerald R.</t>
+  </si>
+  <si>
+    <t>del Riego</t>
+  </si>
+  <si>
+    <t>Rutilio J.</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>McElroy</t>
+  </si>
+  <si>
+    <t>Robert W.</t>
+  </si>
+  <si>
+    <t>http://www.diocese-sdiego.org/</t>
+  </si>
+  <si>
+    <t>Bejarano</t>
+  </si>
+  <si>
+    <t>Ramon</t>
+  </si>
+  <si>
+    <t>Dolan</t>
+  </si>
+  <si>
+    <t>John P.</t>
+  </si>
+  <si>
+    <t>Brom</t>
+  </si>
+  <si>
+    <t>Robert H.</t>
+  </si>
+  <si>
+    <t>San Jose</t>
+  </si>
+  <si>
+    <t>Cantú</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>http://www.dsj.org/</t>
+  </si>
+  <si>
+    <t>McGrath</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Santa Rosa</t>
+  </si>
+  <si>
+    <t>Vasa</t>
+  </si>
+  <si>
+    <t>Robert F.</t>
+  </si>
+  <si>
+    <t>https://srdiocese.org/</t>
+  </si>
+  <si>
+    <t>Walsh</t>
+  </si>
+  <si>
+    <t>Daniel F.</t>
+  </si>
+  <si>
+    <t>Stockton</t>
+  </si>
+  <si>
+    <t>Cotta</t>
+  </si>
+  <si>
+    <t>Myron J.</t>
+  </si>
+  <si>
+    <t>http://www.stocktondiocese.org/</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>@Cassand28566752</t>
+  </si>
+  <si>
+    <t>@Fairbanks_Dioce</t>
+  </si>
+  <si>
+    <t>@PhoenixDiocese</t>
+  </si>
+  <si>
+    <t>@bishopnevares</t>
+  </si>
+  <si>
+    <t>@BishopEdWeisen</t>
+  </si>
+  <si>
+    <t>@dioceseoftucson</t>
   </si>
 </sst>
 </file>
@@ -390,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,6 +660,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,7 +886,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -647,8 +897,8 @@
     <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.0546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
@@ -703,7 +953,7 @@
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -733,7 +983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -763,7 +1013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -815,6 +1065,12 @@
       <c r="G5" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="H5" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="J5" s="9" t="s">
         <v>31</v>
       </c>
@@ -841,6 +1097,12 @@
       <c r="G6" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="H6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="J6" s="9" t="s">
         <v>31</v>
       </c>
@@ -864,6 +1126,12 @@
       <c r="F7" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>167</v>
+      </c>
       <c r="J7" s="5" t="s">
         <v>39</v>
       </c>
@@ -887,6 +1155,13 @@
       <c r="F8" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="J8" s="5" t="s">
         <v>43</v>
       </c>
@@ -910,6 +1185,12 @@
       <c r="F9" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="H9" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="J9" s="5" t="s">
         <v>43</v>
       </c>
@@ -933,6 +1214,12 @@
       <c r="F10" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H10" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>171</v>
+      </c>
       <c r="J10" s="5" t="s">
         <v>50</v>
       </c>
@@ -956,6 +1243,12 @@
       <c r="F11" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="H11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>171</v>
+      </c>
       <c r="J11" s="5" t="s">
         <v>50</v>
       </c>
@@ -1269,122 +1562,660 @@
       <c r="C25" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="D25" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="4"/>
+      <c r="A26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C27" s="4"/>
+      <c r="A27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C28" s="4"/>
+      <c r="A28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="4"/>
+      <c r="A29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C30" s="4"/>
+      <c r="A30" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C31" s="4"/>
+      <c r="A31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A43" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A44" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A45" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A46" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A48" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A50" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A52" s="7" t="s">
+        <v>165</v>
+      </c>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
       <c r="C64" s="4"/>
     </row>
     <row r="65" spans="3:3" ht="12.3" x14ac:dyDescent="0.4">
@@ -4167,8 +4998,35 @@
     <hyperlink ref="J12" r:id="rId11" xr:uid="{4D5A47A4-16F5-4370-834C-F32844B19626}"/>
     <hyperlink ref="J13" r:id="rId12" xr:uid="{DD959C43-40A9-4A46-9260-A8F453E01C2B}"/>
     <hyperlink ref="J14:J24" r:id="rId13" display="http://www.la-archdiocese.org/" xr:uid="{D5AE5C25-2ADB-4C7F-B138-5D1BD4FDEE5A}"/>
+    <hyperlink ref="J25" r:id="rId14" xr:uid="{BB635DB3-4FD3-4757-A744-A9057A5D27AD}"/>
+    <hyperlink ref="J26" r:id="rId15" xr:uid="{E2F179E2-B083-4A3F-B944-5B3F86354E20}"/>
+    <hyperlink ref="J27" r:id="rId16" xr:uid="{17965D47-594E-4F42-8E30-199A342529C0}"/>
+    <hyperlink ref="J28" r:id="rId17" xr:uid="{89AF2A79-5ED2-4EDC-B55B-ED6DF53EF42F}"/>
+    <hyperlink ref="J29" r:id="rId18" xr:uid="{92D45E12-8174-4D4D-96D0-302198B7842D}"/>
+    <hyperlink ref="J30" r:id="rId19" xr:uid="{3C468CAA-18B4-41D5-86AC-F564DEB4853A}"/>
+    <hyperlink ref="J31" r:id="rId20" xr:uid="{A3D8E7AC-3EF3-42CF-ADCF-DB8CF065C6D5}"/>
+    <hyperlink ref="J32" r:id="rId21" xr:uid="{9F1E0407-B54B-4404-BB19-8A8C170A9309}"/>
+    <hyperlink ref="J33" r:id="rId22" xr:uid="{540AFFD1-436B-4302-9814-31E66004E23D}"/>
+    <hyperlink ref="J34" r:id="rId23" xr:uid="{9EE745B1-F004-4E94-9612-3821C0B8AE4B}"/>
+    <hyperlink ref="J35" r:id="rId24" xr:uid="{6F243CC3-D928-480C-867E-D04897DF2ACA}"/>
+    <hyperlink ref="J36" r:id="rId25" xr:uid="{BABD6C51-E4A8-425E-A453-1B0FB7233C69}"/>
+    <hyperlink ref="J37" r:id="rId26" xr:uid="{1D8CB4EB-DE56-40A1-8AEE-645D82A88BD9}"/>
+    <hyperlink ref="J38" r:id="rId27" xr:uid="{0FAA9727-F347-4CB8-A471-F348ABCDCCBE}"/>
+    <hyperlink ref="J39" r:id="rId28" xr:uid="{6EA528FC-91D7-4065-B63B-C2892B7AFAFB}"/>
+    <hyperlink ref="J40" r:id="rId29" xr:uid="{AD621654-5702-415A-9EA6-3B5A30E1035B}"/>
+    <hyperlink ref="J41" r:id="rId30" xr:uid="{AE9F80E1-10A2-44BB-8444-913B6BF22567}"/>
+    <hyperlink ref="J42" r:id="rId31" xr:uid="{4302CF84-0BEF-4FE0-92E3-F61507F0854B}"/>
+    <hyperlink ref="J43" r:id="rId32" xr:uid="{7DDF10EB-5B3C-4514-A6C6-91024B37EC3D}"/>
+    <hyperlink ref="J44" r:id="rId33" xr:uid="{B35C694B-A60F-4C9E-8F09-ABF92E4233AF}"/>
+    <hyperlink ref="J45" r:id="rId34" xr:uid="{9995D4E1-967C-4EE8-8990-72D016D59A98}"/>
+    <hyperlink ref="J46" r:id="rId35" xr:uid="{8312916A-8E79-469C-A729-AD6517A34992}"/>
+    <hyperlink ref="J47" r:id="rId36" xr:uid="{5CDB6D84-5812-4845-8D93-981EE411626F}"/>
+    <hyperlink ref="J48" r:id="rId37" xr:uid="{ECB7BFC9-A7B5-4ABC-9BEF-1D52536E91CF}"/>
+    <hyperlink ref="J49" r:id="rId38" xr:uid="{39065B37-EF40-4525-9776-BB373916C27E}"/>
+    <hyperlink ref="J50" r:id="rId39" xr:uid="{DA437A2A-4334-4B16-B129-820884732A80}"/>
+    <hyperlink ref="J51" r:id="rId40" xr:uid="{AAC7802D-81BD-472C-90A7-71E88D4A57D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>